<commit_message>
Added Supplemental Draft Info
</commit_message>
<xml_diff>
--- a/USFL Schedule.xlsx
+++ b/USFL Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\The-USFL-Data-Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4908A03C-EA68-4B08-9AF2-15A58D4510DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08A3800-6DCC-4027-A729-4C6147C5C0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{EB4FD3FB-8EDB-4A25-8BF0-F4414F55C589}"/>
   </bookViews>
@@ -503,7 +503,7 @@
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>